<commit_message>
Made the sprint 2 backlog
</commit_message>
<xml_diff>
--- a/sprints/Sprint 2/Sprint2Backlog.xlsx
+++ b/sprints/Sprint 2/Sprint2Backlog.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526938E1-D739-4D26-A816-64B2EC93A1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="32130" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,123 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+  <si>
+    <t>Warehouse employee</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>ETA</t>
+  </si>
+  <si>
+    <t>DEADLINE</t>
+  </si>
+  <si>
+    <t>Luke/Carson/Tristen</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>DB redesign</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Update rental status of member order</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Tristen</t>
+  </si>
+  <si>
+    <t>View rental history</t>
+  </si>
+  <si>
+    <t>Carson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View detailed list of orders that are outgoing </t>
+  </si>
+  <si>
+    <t>Manage stock</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>View record of items tracked by which employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress </t>
+  </si>
+  <si>
+    <t>Track when things are received and shipped</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In progress </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +158,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +446,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5">
+        <v>43871</v>
+      </c>
+      <c r="F2" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43860</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43866</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43866</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43866</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43867</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43868</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43869</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the sprint backlog to include development tasks
</commit_message>
<xml_diff>
--- a/sprints/Sprint 2/Sprint2Backlog.xlsx
+++ b/sprints/Sprint 2/Sprint2Backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15082843-1E03-4728-A67B-BE9149DE32AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1BE6D9-3692-4AD6-BED9-65C5FD000A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Warehouse employee</t>
   </si>
@@ -82,9 +82,6 @@
     <t xml:space="preserve">In Progress </t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">In progress </t>
   </si>
   <si>
@@ -92,13 +89,31 @@
   </si>
   <si>
     <t>View detailed list of orders that are outgoing/incoming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement filter for filtering member orders when updating rental status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement SQL queries for gathering all orders made by members for them to view </t>
+  </si>
+  <si>
+    <t>Implement SQL queries for gathering orders of members</t>
+  </si>
+  <si>
+    <t>Design page for customer to view their history</t>
+  </si>
+  <si>
+    <t>Implement SQL queries for gathering information about a single item</t>
+  </si>
+  <si>
+    <t>Design page for manager to view history</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +143,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -158,6 +179,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +496,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -514,7 +536,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -523,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5">
         <v>43866</v>
@@ -534,16 +556,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5">
         <v>43866</v>
@@ -554,16 +576,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5">
         <v>43866</v>
@@ -574,16 +596,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="5">
         <v>43869</v>
@@ -592,41 +614,161 @@
         <v>43873</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43869</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43866</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43873</v>
+      </c>
+    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43866</v>
+      </c>
+      <c r="F10" s="5">
+        <v>43873</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43871</v>
+      </c>
+      <c r="F11" s="5">
+        <v>43873</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43871</v>
+      </c>
+      <c r="F12" s="5">
+        <v>43873</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43869</v>
+      </c>
+      <c r="F13" s="5">
+        <v>43873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>